<commit_message>
Added back creating separate sheets for each group
</commit_message>
<xml_diff>
--- a/Group_Allocator.xlsx
+++ b/Group_Allocator.xlsx
@@ -9,27 +9,27 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10005" windowHeight="7905" tabRatio="870" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10005" windowHeight="7905" tabRatio="870" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="17" r:id="rId1"/>
     <sheet name="Student_Data" sheetId="3" r:id="rId2"/>
     <sheet name="Summary_Results" sheetId="7" r:id="rId3"/>
-    <sheet name="GPA_Chart" sheetId="947" r:id="rId4"/>
-    <sheet name="Gender_Chart" sheetId="948" r:id="rId5"/>
-    <sheet name="Civil_Chart" sheetId="949" r:id="rId6"/>
-    <sheet name="Electrical_Chart" sheetId="950" r:id="rId7"/>
-    <sheet name="CompSys_Chart" sheetId="951" r:id="rId8"/>
-    <sheet name="Software_Chart" sheetId="952" r:id="rId9"/>
-    <sheet name="Mechatronics_Chart" sheetId="953" r:id="rId10"/>
-    <sheet name="Chemmat_Chart" sheetId="954" r:id="rId11"/>
-    <sheet name="Mechanical_Chart" sheetId="955" r:id="rId12"/>
-    <sheet name="Biomedical_Chart" sheetId="956" r:id="rId13"/>
-    <sheet name="EngSci_Chart" sheetId="957" r:id="rId14"/>
-    <sheet name="European(E)_Chart" sheetId="958" r:id="rId15"/>
-    <sheet name="Pacific(E)_Chart" sheetId="959" r:id="rId16"/>
-    <sheet name="Indian(E)_Chart" sheetId="960" r:id="rId17"/>
-    <sheet name="Asian(E)_Chart" sheetId="961" r:id="rId18"/>
+    <sheet name="GPA_Chart" sheetId="1007" r:id="rId4"/>
+    <sheet name="Gender_Chart" sheetId="1008" r:id="rId5"/>
+    <sheet name="Civil_Chart" sheetId="1009" r:id="rId6"/>
+    <sheet name="Electrical_Chart" sheetId="1010" r:id="rId7"/>
+    <sheet name="CompSys_Chart" sheetId="1011" r:id="rId8"/>
+    <sheet name="Software_Chart" sheetId="1012" r:id="rId9"/>
+    <sheet name="Mechatronics_Chart" sheetId="1013" r:id="rId10"/>
+    <sheet name="Chemmat_Chart" sheetId="1014" r:id="rId11"/>
+    <sheet name="Mechanical_Chart" sheetId="1015" r:id="rId12"/>
+    <sheet name="Biomedical_Chart" sheetId="1016" r:id="rId13"/>
+    <sheet name="EngSci_Chart" sheetId="1017" r:id="rId14"/>
+    <sheet name="European(E)_Chart" sheetId="1018" r:id="rId15"/>
+    <sheet name="Pacific(E)_Chart" sheetId="1019" r:id="rId16"/>
+    <sheet name="Indian(E)_Chart" sheetId="1020" r:id="rId17"/>
+    <sheet name="Asian(E)_Chart" sheetId="1021" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="chart_only" localSheetId="1">Student_Data!$K$4</definedName>
@@ -405,9 +405,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Greater than 0?</t>
   </si>
   <si>
@@ -451,6 +448,9 @@
   </si>
   <si>
     <t>When the optimisation has finished running you will automatically be taken to the Summary_Results sheet containing tables of results. You will also find sheets with charts that you can look at to easily see the quality of the solution provided by the optimisation. In addition, a new Excel workbook will have been created and placed in the same directory as this file. This workbook will contain a list of all the groups and the students in each so that you can easily share the allocation with others.</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -972,7 +972,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1539,11 +1538,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="781668496"/>
-        <c:axId val="781675552"/>
+        <c:axId val="452226480"/>
+        <c:axId val="452235104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="781668496"/>
+        <c:axId val="452226480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1565,13 +1564,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="781675552"/>
+        <c:crossAx val="452235104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1579,7 +1577,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="781675552"/>
+        <c:axId val="452235104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -1604,14 +1602,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="781668496"/>
+        <c:crossAx val="452226480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1653,7 +1650,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1818,11 +1814,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="781672808"/>
-        <c:axId val="781678688"/>
+        <c:axId val="462554840"/>
+        <c:axId val="462565032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="781672808"/>
+        <c:axId val="462554840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1844,14 +1840,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="781678688"/>
+        <c:crossAx val="462565032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1859,7 +1854,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="781678688"/>
+        <c:axId val="462565032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -1884,21 +1879,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="781672808"/>
+        <c:crossAx val="462554840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1938,7 +1931,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2103,11 +2095,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="781679472"/>
-        <c:axId val="781670456"/>
+        <c:axId val="462553272"/>
+        <c:axId val="462553664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="781679472"/>
+        <c:axId val="462553272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2129,14 +2121,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="781670456"/>
+        <c:crossAx val="462553664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2144,7 +2135,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="781670456"/>
+        <c:axId val="462553664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -2169,21 +2160,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="781679472"/>
+        <c:crossAx val="462553272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2223,7 +2212,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2388,11 +2376,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="729463096"/>
-        <c:axId val="729475248"/>
+        <c:axId val="462557584"/>
+        <c:axId val="462555232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="729463096"/>
+        <c:axId val="462557584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2414,14 +2402,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="729475248"/>
+        <c:crossAx val="462555232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2429,7 +2416,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="729475248"/>
+        <c:axId val="462555232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -2454,21 +2441,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="729463096"/>
+        <c:crossAx val="462557584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2508,7 +2493,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2673,11 +2657,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="729500336"/>
-        <c:axId val="674044616"/>
+        <c:axId val="462557976"/>
+        <c:axId val="462558368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="729500336"/>
+        <c:axId val="462557976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2699,14 +2683,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="674044616"/>
+        <c:crossAx val="462558368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2714,7 +2697,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="674044616"/>
+        <c:axId val="462558368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -2739,21 +2722,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="729500336"/>
+        <c:crossAx val="462557976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2793,7 +2774,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2958,11 +2938,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="584663768"/>
-        <c:axId val="584664552"/>
+        <c:axId val="462568560"/>
+        <c:axId val="462567776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="584663768"/>
+        <c:axId val="462568560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2984,14 +2964,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="584664552"/>
+        <c:crossAx val="462567776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2999,7 +2978,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="584664552"/>
+        <c:axId val="462567776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -3024,21 +3003,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="584663768"/>
+        <c:crossAx val="462568560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3078,7 +3055,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3243,11 +3219,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="584673960"/>
-        <c:axId val="584671216"/>
+        <c:axId val="462565816"/>
+        <c:axId val="462566208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="584673960"/>
+        <c:axId val="462565816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3269,14 +3245,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="584671216"/>
+        <c:crossAx val="462566208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3284,7 +3259,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="584671216"/>
+        <c:axId val="462566208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -3309,21 +3284,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="584673960"/>
+        <c:crossAx val="462565816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3363,7 +3336,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3674,11 +3646,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="731083616"/>
-        <c:axId val="731084008"/>
+        <c:axId val="452234320"/>
+        <c:axId val="452234712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="731083616"/>
+        <c:axId val="452234320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3700,14 +3672,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="731084008"/>
+        <c:crossAx val="452234712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3715,7 +3686,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="731084008"/>
+        <c:axId val="452234712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -3740,21 +3711,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="731083616"/>
+        <c:crossAx val="452234320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3794,7 +3763,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3959,11 +3927,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="731089888"/>
-        <c:axId val="731090672"/>
+        <c:axId val="462563464"/>
+        <c:axId val="462563072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="731089888"/>
+        <c:axId val="462563464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3985,14 +3953,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="731090672"/>
+        <c:crossAx val="462563072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4000,7 +3967,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="731090672"/>
+        <c:axId val="462563072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -4025,21 +3992,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="731089888"/>
+        <c:crossAx val="462563464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4079,7 +4044,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4244,11 +4208,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="729502296"/>
-        <c:axId val="729494848"/>
+        <c:axId val="462561112"/>
+        <c:axId val="462561504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="729502296"/>
+        <c:axId val="462561112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4270,14 +4234,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="729494848"/>
+        <c:crossAx val="462561504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4285,7 +4248,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="729494848"/>
+        <c:axId val="462561504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -4310,21 +4273,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="729502296"/>
+        <c:crossAx val="462561112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4364,7 +4325,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4529,11 +4489,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="733420424"/>
-        <c:axId val="733423168"/>
+        <c:axId val="462559152"/>
+        <c:axId val="462555624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="733420424"/>
+        <c:axId val="462559152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4555,14 +4515,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="733423168"/>
+        <c:crossAx val="462555624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4570,7 +4529,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="733423168"/>
+        <c:axId val="462555624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -4595,21 +4554,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="733420424"/>
+        <c:crossAx val="462559152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4649,7 +4606,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4814,11 +4770,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="733396512"/>
-        <c:axId val="733410624"/>
+        <c:axId val="462562680"/>
+        <c:axId val="462556408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="733396512"/>
+        <c:axId val="462562680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4840,14 +4796,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="733410624"/>
+        <c:crossAx val="462556408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4855,7 +4810,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="733410624"/>
+        <c:axId val="462556408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -4880,21 +4835,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="733396512"/>
+        <c:crossAx val="462562680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4934,7 +4887,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5099,11 +5051,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="674114416"/>
-        <c:axId val="674106576"/>
+        <c:axId val="462554056"/>
+        <c:axId val="462557192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="674114416"/>
+        <c:axId val="462554056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5125,14 +5077,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="674106576"/>
+        <c:crossAx val="462557192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5140,7 +5091,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="674106576"/>
+        <c:axId val="462557192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -5165,21 +5116,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="674114416"/>
+        <c:crossAx val="462554056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5219,7 +5168,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5384,11 +5332,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="674093248"/>
-        <c:axId val="674095208"/>
+        <c:axId val="462562288"/>
+        <c:axId val="462554448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="674093248"/>
+        <c:axId val="462562288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5410,14 +5358,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="674095208"/>
+        <c:crossAx val="462554448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5425,7 +5372,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="674095208"/>
+        <c:axId val="462554448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -5450,21 +5397,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="674093248"/>
+        <c:crossAx val="462562288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5504,7 +5449,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5669,11 +5613,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="363975416"/>
-        <c:axId val="363974632"/>
+        <c:axId val="462564640"/>
+        <c:axId val="462564248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="363975416"/>
+        <c:axId val="462564640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5695,14 +5639,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="363974632"/>
+        <c:crossAx val="462564248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5710,7 +5653,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="363974632"/>
+        <c:axId val="462564248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -5735,21 +5678,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="363975416"/>
+        <c:crossAx val="462564640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7180,7 +7121,7 @@
       <c r="R3" s="15"/>
       <c r="S3" s="15"/>
       <c r="U3" s="49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="V3" s="50"/>
       <c r="W3" s="50"/>
@@ -7685,7 +7626,7 @@
         <v>36</v>
       </c>
       <c r="B43" s="52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C43" s="53"/>
       <c r="D43" s="53"/>
@@ -7711,7 +7652,7 @@
         <v>37</v>
       </c>
       <c r="B61" s="40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C61" s="41"/>
       <c r="D61" s="41"/>
@@ -7786,7 +7727,7 @@
         <v>38</v>
       </c>
       <c r="B74" s="40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C74" s="41"/>
       <c r="D74" s="41"/>
@@ -7900,8 +7841,8 @@
   </sheetPr>
   <dimension ref="A1:T686"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8031,10 +7972,10 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K4" s="37" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -8379,7 +8320,7 @@
         <v>1.904800810118406</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M15" s="27" t="str">
         <f>IF(K15&gt;0, "Yes", "No")</f>
@@ -8555,7 +8496,7 @@
         <v>4</v>
       </c>
       <c r="J21" s="39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
@@ -8609,7 +8550,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.45">
@@ -8658,7 +8599,7 @@
         <v>1</v>
       </c>
       <c r="J25" s="36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.45">
@@ -8684,10 +8625,10 @@
         <v>3</v>
       </c>
       <c r="J26" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="K26" s="11" t="s">
         <v>85</v>
-      </c>
-      <c r="K26" s="11" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.45">
@@ -8829,7 +8770,7 @@
         <v>16</v>
       </c>
       <c r="J31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -8858,7 +8799,7 @@
         <v>8</v>
       </c>
       <c r="J32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K32">
         <v>1</v>
@@ -8910,7 +8851,7 @@
         <v>12</v>
       </c>
       <c r="J34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.45">
@@ -8936,7 +8877,7 @@
         <v>16</v>
       </c>
       <c r="J35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.45">
@@ -25918,7 +25859,7 @@
     <StoredFile>
       <FileName>Untitled</FileName>
       <LanguageName>PuLP</LanguageName>
-      <ModelPaneVisible>false</ModelPaneVisible>
+      <ModelPaneVisible>true</ModelPaneVisible>
       <ModelSettings/>
       <FileText># ============================================================================
 # Group Allocator - allocates students to balanced groups
@@ -25962,7 +25903,7 @@
 outstanding_gpa_weight = factor_out
 # beta is the number to adjust the upper bound on number of
 # type of people in a group
-beta = 1
+beta = 0
 # The GPA of an 'oustanding' student
 outstanding_gpa = 8.00
 SPECIALISATIONS = list()
@@ -26731,41 +26672,35 @@
         Application.DisplayAlerts = False
         sheet.Delete()
         Application.DisplayAlerts = True
-# Make a sheet for each group
-# for g in GROUPS:
-#     count = Application.Worksheets.Count
-#     wb.Sheets.Add(After=wb.Sheets(count))
-#     wb_name = 'Group_%s' % g
-#     wb.ActiveSheet.Name = wb_name
-#     ws = wb.Worksheets(wb_name)
-#     # Headers
-#     ws.Cells(1, 1).Value = 'Group'
-#     ws.Cells(1, 1).Font.Bold = True
-#     ws.Cells(1, 2).Value = 'Name'
-#     ws.Cells(1, 2).Font.Bold = True
-#     ws.Cells(1, 3).Value = 'Gender'
-#     ws.Cells(1, 3).Font.Bold = True
-#     ws.Cells(1, 4).Value = 'UPI'
-#     ws.Cells(1, 4).Font.Bold = True
-#     ws.Cells(1, 5).Value = 'Discipline'
-#     ws.Cells(1, 5).Font.Bold = True
-#     ws.Cells(1, 6).Value = 'UoA Email'
-#     ws.Cells(1, 6).Font.Bold = True
-#     # Data
-#     row_index = 1
-#     for s in students_in_group[g]:
-#         row_index += 1
-#         ws.Cells(row_index, 1).Value = g
-#         ws.Cells(row_index, 2).Value = NAMES[s]
-#         ws.Cells(row_index, 3).Value = gender[s]
-#         ws.Cells(row_index, 4).Value = UPI[s]
-#         ws.Cells(row_index, 5).Value = specialisation[s]
-#         ws.Cells(row_index, 6).Value = '%s@aucklanduni.ac.nz' % UPI[s]
-#     # Activate
-#     ws.Activate()
-#     ws.Cells.Select()
-#     Application.Selection.Columns.AutoFit()
-#     ws.Cells(1, 1).Select()
+#Make a sheet for each group
+for g in GROUPS:
+    count = Application.Worksheets.Count
+    wb.Sheets.Add(After=wb.Sheets(count))
+    wb_name = 'Group_%s' % g
+    wb.ActiveSheet.Name = wb_name
+    ws = wb.Worksheets(wb_name)
+    # Headers
+    ws.Cells(1, 1).Value = 'Group'
+    ws.Cells(1, 1).Font.Bold = True
+    ws.Cells(1, 2).Value = 'Name'
+    ws.Cells(1, 2).Font.Bold = True
+    ws.Cells(1, 3).Value = 'Discipline'
+    ws.Cells(1, 3).Font.Bold = True
+    ws.Cells(1, 4).Value = 'UoA Email'
+    ws.Cells(1, 4).Font.Bold = True
+    # Data
+    row_index = 1
+    for s in students_in_group[g]:
+        row_index += 1
+        ws.Cells(row_index, 1).Value = g
+        ws.Cells(row_index, 2).Value = NAMES[s]
+        ws.Cells(row_index, 3).Value = specialisation[s]
+        ws.Cells(row_index, 4).Value = '%s@aucklanduni.ac.nz' % UPI[s]
+    # Activate
+    ws.Activate()
+    ws.Cells.Select()
+    Application.Selection.Columns.AutoFit()
+    ws.Cells(1, 1).Select()
 wb.Worksheets('All_Groups').Activate()
 wb.Save()
 </FileText>
@@ -26782,7 +26717,7 @@
     <StoredFile>
       <FileName>Untitled</FileName>
       <LanguageName>PuLP</LanguageName>
-      <ModelPaneVisible>false</ModelPaneVisible>
+      <ModelPaneVisible>true</ModelPaneVisible>
       <ModelSettings/>
       <FileText>a = Application.ActiveChart
 xlY = 1
@@ -26808,7 +26743,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD451F4C-196B-43E8-923D-68901783E891}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0CD35C9-69A0-4F79-9A2E-F2DB9DD21665}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://opensolver.org"/>

</xml_diff>

<commit_message>
Added upi back to group list output
</commit_message>
<xml_diff>
--- a/Group_Allocator.xlsx
+++ b/Group_Allocator.xlsx
@@ -16,21 +16,21 @@
     <sheet name="AboutSupport" sheetId="1052" r:id="rId2"/>
     <sheet name="Student_Data" sheetId="3" r:id="rId3"/>
     <sheet name="Summary_Results" sheetId="7" r:id="rId4"/>
-    <sheet name="GPA_Chart" sheetId="1054" r:id="rId5"/>
-    <sheet name="Gender_Chart" sheetId="1055" r:id="rId6"/>
-    <sheet name="Civil_Chart" sheetId="1056" r:id="rId7"/>
-    <sheet name="Electrical_Chart" sheetId="1057" r:id="rId8"/>
-    <sheet name="CompSys_Chart" sheetId="1058" r:id="rId9"/>
-    <sheet name="Software_Chart" sheetId="1059" r:id="rId10"/>
-    <sheet name="Mechatronics_Chart" sheetId="1060" r:id="rId11"/>
-    <sheet name="Chemmat_Chart" sheetId="1061" r:id="rId12"/>
-    <sheet name="Mechanical_Chart" sheetId="1062" r:id="rId13"/>
-    <sheet name="Biomedical_Chart" sheetId="1063" r:id="rId14"/>
-    <sheet name="EngSci_Chart" sheetId="1064" r:id="rId15"/>
-    <sheet name="European(E)_Chart" sheetId="1065" r:id="rId16"/>
-    <sheet name="Pacific(E)_Chart" sheetId="1066" r:id="rId17"/>
-    <sheet name="Indian(E)_Chart" sheetId="1067" r:id="rId18"/>
-    <sheet name="Asian(E)_Chart" sheetId="1068" r:id="rId19"/>
+    <sheet name="GPA_Chart" sheetId="1069" r:id="rId5"/>
+    <sheet name="Gender_Chart" sheetId="1070" r:id="rId6"/>
+    <sheet name="Civil_Chart" sheetId="1071" r:id="rId7"/>
+    <sheet name="Electrical_Chart" sheetId="1072" r:id="rId8"/>
+    <sheet name="CompSys_Chart" sheetId="1073" r:id="rId9"/>
+    <sheet name="Software_Chart" sheetId="1074" r:id="rId10"/>
+    <sheet name="Mechatronics_Chart" sheetId="1075" r:id="rId11"/>
+    <sheet name="Chemmat_Chart" sheetId="1076" r:id="rId12"/>
+    <sheet name="Mechanical_Chart" sheetId="1077" r:id="rId13"/>
+    <sheet name="Biomedical_Chart" sheetId="1078" r:id="rId14"/>
+    <sheet name="EngSci_Chart" sheetId="1079" r:id="rId15"/>
+    <sheet name="European(E)_Chart" sheetId="1080" r:id="rId16"/>
+    <sheet name="Pacific(E)_Chart" sheetId="1081" r:id="rId17"/>
+    <sheet name="Indian(E)_Chart" sheetId="1082" r:id="rId18"/>
+    <sheet name="Asian(E)_Chart" sheetId="1083" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Student_Data!$A$1:$H$686</definedName>
@@ -868,6 +868,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -879,6 +891,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -894,27 +915,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1015,6 +1015,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1581,11 +1582,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="445443064"/>
-        <c:axId val="445447376"/>
+        <c:axId val="695763312"/>
+        <c:axId val="695764488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="445443064"/>
+        <c:axId val="695763312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1607,12 +1608,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445447376"/>
+        <c:crossAx val="695764488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1620,7 +1622,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="445447376"/>
+        <c:axId val="695764488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -1645,13 +1647,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445443064"/>
+        <c:crossAx val="695763312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1693,6 +1696,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1857,11 +1861,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="456003256"/>
-        <c:axId val="455996592"/>
+        <c:axId val="701896032"/>
+        <c:axId val="701887408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="456003256"/>
+        <c:axId val="701896032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1883,13 +1887,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455996592"/>
+        <c:crossAx val="701887408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1897,7 +1902,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455996592"/>
+        <c:axId val="701887408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -1922,19 +1927,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="456003256"/>
+        <c:crossAx val="701896032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1974,6 +1981,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2138,11 +2146,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="455994240"/>
-        <c:axId val="456001688"/>
+        <c:axId val="696731960"/>
+        <c:axId val="696732352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455994240"/>
+        <c:axId val="696731960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2164,13 +2172,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="456001688"/>
+        <c:crossAx val="696732352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2178,7 +2187,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="456001688"/>
+        <c:axId val="696732352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -2203,19 +2212,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455994240"/>
+        <c:crossAx val="696731960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2255,6 +2266,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2419,11 +2431,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="455998552"/>
-        <c:axId val="455997376"/>
+        <c:axId val="696742544"/>
+        <c:axId val="696735880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455998552"/>
+        <c:axId val="696742544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2445,13 +2457,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455997376"/>
+        <c:crossAx val="696735880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2459,7 +2472,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455997376"/>
+        <c:axId val="696735880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -2484,19 +2497,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455998552"/>
+        <c:crossAx val="696742544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2536,6 +2551,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2700,11 +2716,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="455998160"/>
-        <c:axId val="455999336"/>
+        <c:axId val="696747248"/>
+        <c:axId val="696750776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455998160"/>
+        <c:axId val="696747248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2726,13 +2742,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455999336"/>
+        <c:crossAx val="696750776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2740,7 +2757,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455999336"/>
+        <c:axId val="696750776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -2765,19 +2782,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455998160"/>
+        <c:crossAx val="696747248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2817,6 +2836,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2981,11 +3001,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="455996984"/>
-        <c:axId val="455995024"/>
+        <c:axId val="696753520"/>
+        <c:axId val="696748032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455996984"/>
+        <c:axId val="696753520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3007,13 +3027,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455995024"/>
+        <c:crossAx val="696748032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3021,7 +3042,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455995024"/>
+        <c:axId val="696748032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -3046,19 +3067,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455996984"/>
+        <c:crossAx val="696753520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3098,6 +3121,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3262,11 +3286,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="456003648"/>
-        <c:axId val="455998944"/>
+        <c:axId val="696759008"/>
+        <c:axId val="696759400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="456003648"/>
+        <c:axId val="696759008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3288,13 +3312,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455998944"/>
+        <c:crossAx val="696759400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3302,7 +3327,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455998944"/>
+        <c:axId val="696759400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -3327,19 +3352,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="456003648"/>
+        <c:crossAx val="696759008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3379,6 +3406,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3689,11 +3717,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="445445416"/>
-        <c:axId val="445450904"/>
+        <c:axId val="695748416"/>
+        <c:axId val="695755864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="445445416"/>
+        <c:axId val="695748416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3715,13 +3743,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445450904"/>
+        <c:crossAx val="695755864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3729,7 +3758,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="445450904"/>
+        <c:axId val="695755864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -3754,19 +3783,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445445416"/>
+        <c:crossAx val="695748416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3806,6 +3837,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3970,11 +4002,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="445451688"/>
-        <c:axId val="445439928"/>
+        <c:axId val="695751944"/>
+        <c:axId val="695750376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="445451688"/>
+        <c:axId val="695751944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3996,13 +4028,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445439928"/>
+        <c:crossAx val="695750376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4010,7 +4043,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="445439928"/>
+        <c:axId val="695750376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -4035,19 +4068,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445451688"/>
+        <c:crossAx val="695751944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4087,6 +4122,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4251,11 +4287,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="445443456"/>
-        <c:axId val="445446592"/>
+        <c:axId val="695749592"/>
+        <c:axId val="695749984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="445443456"/>
+        <c:axId val="695749592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4277,13 +4313,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445446592"/>
+        <c:crossAx val="695749984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4291,7 +4328,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="445446592"/>
+        <c:axId val="695749984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -4316,19 +4353,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445443456"/>
+        <c:crossAx val="695749592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4368,6 +4407,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4532,11 +4572,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="445444632"/>
-        <c:axId val="445453648"/>
+        <c:axId val="695755472"/>
+        <c:axId val="711122296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="445444632"/>
+        <c:axId val="695755472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4558,13 +4598,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445453648"/>
+        <c:crossAx val="711122296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4572,7 +4613,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="445453648"/>
+        <c:axId val="711122296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -4597,19 +4638,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445444632"/>
+        <c:crossAx val="695755472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4649,6 +4692,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4813,11 +4857,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="445454432"/>
-        <c:axId val="445454824"/>
+        <c:axId val="701896424"/>
+        <c:axId val="701888192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="445454432"/>
+        <c:axId val="701896424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4839,13 +4883,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445454824"/>
+        <c:crossAx val="701888192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4853,7 +4898,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="445454824"/>
+        <c:axId val="701888192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -4878,19 +4923,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445454432"/>
+        <c:crossAx val="701896424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4930,6 +4977,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5094,11 +5142,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="445441104"/>
-        <c:axId val="445442280"/>
+        <c:axId val="701907400"/>
+        <c:axId val="701905440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="445441104"/>
+        <c:axId val="701907400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5120,13 +5168,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445442280"/>
+        <c:crossAx val="701905440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5134,7 +5183,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="445442280"/>
+        <c:axId val="701905440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -5159,19 +5208,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445441104"/>
+        <c:crossAx val="701907400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5211,6 +5262,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5375,11 +5427,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="445455216"/>
-        <c:axId val="445455608"/>
+        <c:axId val="701899560"/>
+        <c:axId val="701899952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="445455216"/>
+        <c:axId val="701899560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5401,13 +5453,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445455608"/>
+        <c:crossAx val="701899952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5415,7 +5468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="445455608"/>
+        <c:axId val="701899952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -5440,19 +5493,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445455216"/>
+        <c:crossAx val="701899560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5492,6 +5547,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5656,11 +5712,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="445453256"/>
-        <c:axId val="445444240"/>
+        <c:axId val="701914848"/>
+        <c:axId val="701910144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="445453256"/>
+        <c:axId val="701914848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5682,13 +5738,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445444240"/>
+        <c:crossAx val="701910144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5696,7 +5753,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="445444240"/>
+        <c:axId val="701910144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -5721,19 +5778,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="445453256"/>
+        <c:crossAx val="701914848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6861,20 +6920,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="26.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="44"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="48"/>
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
@@ -6887,61 +6946,61 @@
     </row>
     <row r="2" spans="1:19" ht="14.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="1:19" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="52"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="51"/>
     </row>
     <row r="18" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="19" spans="1:24" ht="14.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="20" spans="1:24" ht="88.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="52"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="51"/>
     </row>
     <row r="25" spans="1:24" ht="14.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="26" spans="1:24" ht="149.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="56" t="s">
+      <c r="A26" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="52"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="51"/>
     </row>
     <row r="32" spans="1:24" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="U32" s="41"/>
-      <c r="V32" s="41"/>
-      <c r="W32" s="41"/>
-      <c r="X32" s="41"/>
+      <c r="U32" s="45"/>
+      <c r="V32" s="45"/>
+      <c r="W32" s="45"/>
+      <c r="X32" s="45"/>
     </row>
     <row r="33" spans="1:24" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="U33" s="36"/>
@@ -7014,20 +7073,20 @@
       <c r="J44" s="21"/>
     </row>
     <row r="45" spans="1:24" ht="98.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="56" t="s">
+      <c r="A45" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="53" t="s">
+      <c r="B45" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="C45" s="54"/>
-      <c r="D45" s="54"/>
-      <c r="E45" s="54"/>
-      <c r="F45" s="54"/>
-      <c r="G45" s="54"/>
-      <c r="H45" s="54"/>
-      <c r="I45" s="54"/>
-      <c r="J45" s="55"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="44"/>
     </row>
     <row r="46" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B46" s="21"/>
@@ -7151,20 +7210,20 @@
       <c r="J56" s="21"/>
     </row>
     <row r="57" spans="1:11" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A57" s="56" t="s">
+      <c r="A57" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="53" t="s">
+      <c r="B57" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C57" s="54"/>
-      <c r="D57" s="54"/>
-      <c r="E57" s="54"/>
-      <c r="F57" s="54"/>
-      <c r="G57" s="54"/>
-      <c r="H57" s="54"/>
-      <c r="I57" s="54"/>
-      <c r="J57" s="55"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="44"/>
     </row>
     <row r="58" spans="1:11" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B58" s="21"/>
@@ -7304,62 +7363,62 @@
       <c r="L1" s="17"/>
     </row>
     <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="47"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="54"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="47"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="54"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="47"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="54"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="47"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="54"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="40"/>
@@ -7462,27 +7521,27 @@
       <c r="L11" s="10"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
     </row>
     <row r="14" spans="1:12" ht="49.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -26314,12 +26373,12 @@
 ws.Cells(1, 2).Font.Bold = True
 # ws.Cells(1, 3).Value = 'Gender'
 # ws.Cells(1, 3).Font.Bold = True
-# ws.Cells(1, 3).Value = 'UPI'
-# ws.Cells(1, 3).Font.Bold = True
-ws.Cells(1, 3).Value = 'Discipline'
+ws.Cells(1, 3).Value = 'UPI'
 ws.Cells(1, 3).Font.Bold = True
-ws.Cells(1, 4).Value = 'Email'
+ws.Cells(1, 4).Value = 'Discipline'
 ws.Cells(1, 4).Font.Bold = True
+ws.Cells(1, 5).Value = 'UoA Email'
+ws.Cells(1, 5).Font.Bold = True
 # Data
 row_index = 1
 for g in GROUPS:
@@ -26328,9 +26387,9 @@
         ws.Cells(row_index, 1).Value = g
         ws.Cells(row_index, 2).Value = NAMES[s]
         # ws.Cells(row_index, 3).Value = gender[s]
-        # ws.Cells(row_index, 3).Value = UPI[s]
-        ws.Cells(row_index, 3).Value = specialisation[s]
-        ws.Cells(row_index, 4).Value = '%s@aucklanduni.ac.nz' % UPI[s]
+        ws.Cells(row_index, 3).Value = UPI[s]
+        ws.Cells(row_index, 4).Value = specialisation[s]
+        ws.Cells(row_index, 5).Value = '%s@aucklanduni.ac.nz' % UPI[s]
         # Space between each group
     #row_index += 1
 ws.Activate()
@@ -26354,18 +26413,21 @@
     ws.Cells(1, 1).Font.Bold = True
     ws.Cells(1, 2).Value = 'Name'
     ws.Cells(1, 2).Font.Bold = True
-    ws.Cells(1, 3).Value = 'Discipline'
+    ws.Cells(1, 3).Value = 'UPI'
     ws.Cells(1, 3).Font.Bold = True
-    ws.Cells(1, 4).Value = 'UoA Email'
+    ws.Cells(1, 4).Value = 'Discipline'
     ws.Cells(1, 4).Font.Bold = True
+    ws.Cells(1, 5).Value = 'UoA Email'
+    ws.Cells(1, 5).Font.Bold = True
     # Data
     row_index = 1
     for s in students_in_group[g]:
         row_index += 1
         ws.Cells(row_index, 1).Value = g
         ws.Cells(row_index, 2).Value = NAMES[s]
-        ws.Cells(row_index, 3).Value = specialisation[s]
-        ws.Cells(row_index, 4).Value = '%s@aucklanduni.ac.nz' % UPI[s]
+        ws.Cells(row_index, 3).Value = UPI[s]
+        ws.Cells(row_index, 4).Value = specialisation[s]
+        ws.Cells(row_index, 5).Value = '%s@aucklanduni.ac.nz' % UPI[s]
     # Activate
     ws.Activate()
     ws.Cells.Select()
@@ -26421,7 +26483,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1DBD013-4D4D-48D8-B223-C7DE367E96CF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87204D52-C514-42D4-BFB6-7B1AB7087945}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://opensolver.org"/>

</xml_diff>